<commit_message>
update on add xlsx on db
</commit_message>
<xml_diff>
--- a/Solde CP.xlsx
+++ b/Solde CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\PING_2019_And\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EFF3E6-546D-402B-B14A-82859DA84697}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240AA828-9BA0-45F1-B29F-FE022014FC9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8952" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="55">
   <si>
     <t>Solde des repos  - Mars 2019</t>
   </si>
@@ -79,9 +79,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>0000000087</t>
-  </si>
-  <si>
     <t>0000000104</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
   </si>
   <si>
     <t>0000000107</t>
-  </si>
-  <si>
-    <t>0000000085</t>
   </si>
   <si>
     <t>0000000071</t>
@@ -1141,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1272,8 +1266,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
+      <c r="A6" s="2">
+        <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
@@ -1308,7 +1302,7 @@
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
@@ -1343,7 +1337,7 @@
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
@@ -1378,7 +1372,7 @@
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
@@ -1413,7 +1407,7 @@
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>15</v>
@@ -1448,7 +1442,7 @@
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
@@ -1483,7 +1477,7 @@
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>15</v>
@@ -1518,7 +1512,7 @@
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
@@ -1552,8 +1546,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>24</v>
+      <c r="A14" s="2">
+        <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
@@ -1588,7 +1582,7 @@
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -1623,7 +1617,7 @@
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
@@ -1658,7 +1652,7 @@
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
@@ -1693,7 +1687,7 @@
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>15</v>
@@ -1728,7 +1722,7 @@
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>15</v>
@@ -1763,7 +1757,7 @@
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>15</v>
@@ -1798,7 +1792,7 @@
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>15</v>
@@ -1833,7 +1827,7 @@
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>15</v>
@@ -1868,7 +1862,7 @@
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>15</v>
@@ -1903,7 +1897,7 @@
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>15</v>
@@ -1938,7 +1932,7 @@
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>15</v>
@@ -1973,7 +1967,7 @@
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>15</v>
@@ -2008,7 +2002,7 @@
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>15</v>
@@ -2043,7 +2037,7 @@
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>15</v>
@@ -2078,7 +2072,7 @@
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>15</v>
@@ -2113,7 +2107,7 @@
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>15</v>
@@ -2148,7 +2142,7 @@
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>15</v>
@@ -2183,7 +2177,7 @@
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>15</v>
@@ -2218,7 +2212,7 @@
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>15</v>
@@ -2253,7 +2247,7 @@
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>15</v>
@@ -2288,7 +2282,7 @@
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>15</v>
@@ -2323,7 +2317,7 @@
     </row>
     <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>15</v>
@@ -2358,7 +2352,7 @@
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>15</v>
@@ -2393,7 +2387,7 @@
     </row>
     <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>15</v>
@@ -2428,7 +2422,7 @@
     </row>
     <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>15</v>
@@ -2463,7 +2457,7 @@
     </row>
     <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>15</v>
@@ -2498,7 +2492,7 @@
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>15</v>
@@ -2533,7 +2527,7 @@
     </row>
     <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>15</v>
@@ -2568,7 +2562,7 @@
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>15</v>
@@ -2603,7 +2597,7 @@
     </row>
     <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>15</v>
@@ -2638,7 +2632,7 @@
     </row>
     <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>15</v>
@@ -2676,7 +2670,7 @@
         <v>14</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C46" s="6">
         <v>343.47</v>

</xml_diff>